<commit_message>
added ink! code snippets
</commit_message>
<xml_diff>
--- a/polkadot_vs_eosio_vs_evm.xlsx
+++ b/polkadot_vs_eosio_vs_evm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhi3700/F/coding/github_repos/My_Learning_Polkadot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDBBC24-E307-9B43-9533-8BE37B7E3767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B342100F-D828-CA46-A5D7-4B4F5E50284E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14320" xr2:uid="{525611D5-18D7-41F8-A371-26E5FA616275}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="144">
   <si>
     <t>EOSIO</t>
   </si>
@@ -652,22 +652,25 @@
     <t>SC language (natively supported)</t>
   </si>
   <si>
-    <t>Solidity, Vyper</t>
-  </si>
-  <si>
     <t>eDSL</t>
   </si>
   <si>
     <t>ink!</t>
   </si>
   <si>
-    <t>eosio</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>A language developed on top of main language</t>
+  </si>
+  <si>
+    <t>eosio C++</t>
+  </si>
+  <si>
+    <t>Solidity, Vyper, Fe</t>
+  </si>
+  <si>
+    <t>Self::env().caller</t>
   </si>
 </sst>
 </file>
@@ -758,7 +761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -770,9 +773,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -897,7 +897,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1185,7 +1185,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E29F14-69FA-4A1C-8576-9B2A132A653B}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,25 +1238,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1378,19 +1378,19 @@
     </row>
     <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1407,7 +1407,7 @@
         <v>135</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1440,7 +1440,9 @@
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
@@ -1454,7 +1456,7 @@
       <c r="G12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1761,10 +1763,10 @@
         <v>106</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>117</v>
       </c>
       <c r="E29" s="2" t="s">

</xml_diff>